<commit_message>
use cameCase for asset properties
</commit_message>
<xml_diff>
--- a/tests/data/asset-architect-test.xlsx
+++ b/tests/data/asset-architect-test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29428175-9761-C947-B3DC-C6910EBD6AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C817702-897D-D449-B778-932593564CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="32900" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Data Model Properties</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>cim:Terminal</t>
+  </si>
+  <si>
+    <t>cim:Terminal(cim:mRID)</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,7 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -8681,7 +8684,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9922,8 +9925,8 @@
   </sheetPr>
   <dimension ref="A1:W909"/>
   <sheetViews>
-    <sheetView zoomScale="131" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9934,7 +9937,7 @@
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.5" style="8" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="80.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="40.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="62.1640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -10018,7 +10021,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>43</v>
@@ -16430,5 +16433,6 @@
     <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Neat 371 relationship loader (#554)
* scoping of asset loader

* add write_to_file

* use cameCase for asset properties

* fix failing tests

* fix test

* making sure we do not create asset whose parent does not exist

* making sure we do not create asset whose parent does not exist

* orphage test

* bump version add changelog

* update change log [skip ci]

* push changes

* fix py

* added some extras

* finalize relationship loader

* fix tests

* merge asset and relationship loader

* remove unecessary test file

* fix write to file

* bump version

* added missing capabilities [skip ci]

* Update cognite/neat/graph/loaders/_rdf2asset.py

Co-authored-by: Anders Albert <60234212+doctrino@users.noreply.github.com>

* Update cognite/neat/graph/loaders/_rdf2asset.py

Co-authored-by: Anders Albert <60234212+doctrino@users.noreply.github.com>

---------

Co-authored-by: Anders Albert <60234212+doctrino@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/data/asset-architect-test.xlsx
+++ b/tests/data/asset-architect-test.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/Repos/neat/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C817702-897D-D449-B778-932593564CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ECB3282-C99B-7E49-9D22-FB78C8C2400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17800" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Classes" sheetId="2" r:id="rId2"/>
     <sheet name="Properties" sheetId="3" r:id="rId3"/>
+    <sheet name="Prefixes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="93">
   <si>
     <t>Data Model Properties</t>
   </si>
@@ -129,22 +130,334 @@
     <t>GeographicalRegion</t>
   </si>
   <si>
-    <t>RootCIMNode</t>
+    <t>Transformation</t>
   </si>
   <si>
-    <t>Analog</t>
+    <t>Prefix</t>
   </si>
   <si>
-    <t>Orphanage</t>
+    <t>URI</t>
   </si>
   <si>
-    <t>Transformation</t>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
+  </si>
+  <si>
+    <t>rdfs</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#</t>
+  </si>
+  <si>
+    <t>dct</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/terms/</t>
   </si>
   <si>
     <t>cim</t>
   </si>
   <si>
     <t>http://iec.ch/TC57/2013/CIM-schema-cim16#</t>
+  </si>
+  <si>
+    <t>icim</t>
+  </si>
+  <si>
+    <t>http://iec.ch/TC57/2013/CIM-schema-cim16-info#</t>
+  </si>
+  <si>
+    <t>entsoe</t>
+  </si>
+  <si>
+    <t>http://entsoe.eu/CIM/SchemaExtension/3/1#</t>
+  </si>
+  <si>
+    <t>entsoe2</t>
+  </si>
+  <si>
+    <t>http://entsoe.eu/CIM/SchemaExtension/3/2#</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t>http://iec.ch/TC57/61970-552/ModelDescription/1#</t>
+  </si>
+  <si>
+    <t>pti</t>
+  </si>
+  <si>
+    <t>http://www.pti-us.com/PTI_CIM-schema-cim16#</t>
+  </si>
+  <si>
+    <t>nordic44</t>
+  </si>
+  <si>
+    <t>http://purl.org/nordic44#</t>
+  </si>
+  <si>
+    <r>
+      <t>Prefix/URI for Resource Description Framework (RDF) which is base for all RDF statements both in data model and knowledge graph. Learn more:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.w3.org/TR/rdf11-primer/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for RDF Schema vocabulary (RDFS). RDFS provides a data-modelling vocabulary for RDF data. RDF Schema is an extension of the basic RDF vocabulary. Learn more: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>https://www.w3.org/TR/rdf-schema/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Dublin Core (Terms) Metadata Terms</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> which terms such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>title</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>description</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>rights</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>source</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">, etc. we will use to describe our data model. Learn more: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>https://en.wikipedia.org/wiki/Dublin_Core</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for Entsoe Schedule Market Extension of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">CIM 16  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>which defines classes which are used (instantiated) in for example Nordic44 knowledge graph.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for Entose Extension of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">CIM 16  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>which defines classes which are used (instantiated) in for example Nordic44 knowledge graph.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for Entose Extension of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>CIM 16</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">CIM 16 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>model exchange format.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Prefix/URI for Siemens </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">CIM 16 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>extension.</t>
+    </r>
+  </si>
+  <si>
+    <t>This is prefix which is used when loading Nordic44 to triple store.</t>
   </si>
   <si>
     <t>Jimbo</t>
@@ -180,17 +493,53 @@
     <t>connectivityNode</t>
   </si>
   <si>
+    <t>VoltageLevel</t>
+  </si>
+  <si>
+    <t>ConnectivityNode</t>
+  </si>
+  <si>
+    <t>Asset(property=parentExternalId), Relationship</t>
+  </si>
+  <si>
+    <t>voltageLevel</t>
+  </si>
+  <si>
+    <t>cim:ConnectivityNode(cim:IdentifiedObject.description)</t>
+  </si>
+  <si>
+    <t>cim:ConnectivityNode(cim:ConnectivityNode.ConnectivityNodeContainer)</t>
+  </si>
+  <si>
+    <t>cim:VoltageLevel(cim:IdentifiedObject.description)</t>
+  </si>
+  <si>
+    <t>substation</t>
+  </si>
+  <si>
+    <t>cim:VoltageLevel(cim:VoltageLevel.Substation)</t>
+  </si>
+  <si>
+    <t>cim:Substation(cim:IdentifiedObject.description)</t>
+  </si>
+  <si>
     <t>cim:Terminal</t>
   </si>
   <si>
-    <t>cim:Terminal(cim:mRID)</t>
+    <t>cim:ConnectivityNode</t>
+  </si>
+  <si>
+    <t>cim:VoltageLevel</t>
+  </si>
+  <si>
+    <t>cim:Substation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,6 +630,49 @@
       <name val="Aptos Narrow"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,7 +699,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -393,11 +785,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -474,16 +881,34 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -495,6 +920,9 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,8 +1231,8 @@
   </sheetPr>
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -838,7 +1266,7 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -850,7 +1278,7 @@
         <v>18</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="18"/>
@@ -907,8 +1335,8 @@
       <c r="A6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>40</v>
+      <c r="B6" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -936,8 +1364,8 @@
       <c r="A7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>39</v>
+      <c r="B7" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -8681,10 +9109,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView zoomScale="170" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8698,13 +9126,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -8728,25 +9156,25 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="10"/>
@@ -8764,7 +9192,7 @@
     </row>
     <row r="5" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -8773,7 +9201,7 @@
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -8782,7 +9210,7 @@
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -8791,7 +9219,7 @@
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -8799,9 +9227,7 @@
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -8839,7 +9265,7 @@
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8860,21 +9286,21 @@
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="14"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="12"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8902,7 +9328,7 @@
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="12"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8926,26 +9352,20 @@
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
     </row>
-    <row r="27" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
     </row>
-    <row r="28" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-    </row>
+    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9909,7 +10329,6 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
@@ -9923,21 +10342,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W909"/>
+  <dimension ref="A1:W908"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="131" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="7" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="40.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="8" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="8" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="63.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="62.1640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="46.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -9945,18 +10364,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -9991,10 +10410,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -10003,12 +10422,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10" t="s">
@@ -10021,20 +10440,20 @@
         <v>1</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
@@ -10047,20 +10466,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
@@ -10073,24 +10492,24 @@
         <v>1</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>51</v>
+      <c r="B6" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="E6" s="24">
         <v>0</v>
@@ -10099,190 +10518,375 @@
         <v>1</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="24">
+        <v>1</v>
+      </c>
+      <c r="F7" s="24">
+        <v>1</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="24">
+        <v>1</v>
+      </c>
+      <c r="F8" s="24">
+        <v>1</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+      <c r="F9" s="24">
+        <v>1</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="24">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24">
+        <v>1</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="24">
+        <v>1</v>
+      </c>
+      <c r="F11" s="24">
+        <v>1</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="24">
+        <v>1</v>
+      </c>
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+      <c r="F14" s="24">
+        <v>1</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="24">
+        <v>1</v>
+      </c>
+      <c r="F15" s="24">
+        <v>1</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="24">
+        <v>1</v>
+      </c>
+      <c r="F16" s="24">
+        <v>1</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="24">
+        <v>0</v>
+      </c>
+      <c r="F17" s="24">
+        <v>1</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
     </row>
-    <row r="20" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-    </row>
-    <row r="23" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-    </row>
-    <row r="26" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
     </row>
-    <row r="28" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C30" s="5"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
@@ -16420,13 +17024,6 @@
       <c r="F908" s="6"/>
       <c r="G908" s="6"/>
       <c r="H908" s="6"/>
-    </row>
-    <row r="909" spans="3:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C909" s="5"/>
-      <c r="E909" s="6"/>
-      <c r="F909" s="6"/>
-      <c r="G909" s="6"/>
-      <c r="H909" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -16435,4 +17032,139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEC69AD-6A47-8A49-AB04-004D0BC3921D}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="23" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>